<commit_message>
corrected a bug in stopping criterion of KSVD - moved the computation of avg error in each iteration after dictionary is cleared
</commit_message>
<xml_diff>
--- a/output/to_publish/results6.xlsx
+++ b/output/to_publish/results6.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="25">
   <si>
     <t>Dataset name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Stop criterion</t>
+  </si>
+  <si>
+    <t>dl</t>
   </si>
 </sst>
 </file>
@@ -961,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,7 +1141,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1">
         <v>1500</v>
@@ -1149,29 +1152,21 @@
       <c r="E5" s="3">
         <v>1.3956200000000001</v>
       </c>
-      <c r="F5" s="1">
-        <v>587</v>
-      </c>
-      <c r="G5" s="1">
-        <v>1500000</v>
-      </c>
-      <c r="H5" s="1">
-        <v>590983</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.39399000000000001</v>
-      </c>
-      <c r="J5" s="1">
-        <v>10</v>
-      </c>
-      <c r="K5" s="3">
-        <v>2.0233300000000001</v>
-      </c>
-      <c r="L5" s="3">
-        <v>1.39554</v>
-      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="3"/>
       <c r="M5" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>15</v>
@@ -1182,7 +1177,7 @@
         <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>1500</v>
@@ -1193,29 +1188,21 @@
       <c r="E6" s="3">
         <v>1.3956200000000001</v>
       </c>
-      <c r="F6" s="1">
-        <v>174</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1500000</v>
-      </c>
-      <c r="H6" s="1">
-        <v>180570</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.12038</v>
-      </c>
-      <c r="J6" s="1">
-        <v>3</v>
-      </c>
-      <c r="K6" s="6">
-        <v>2.7480000000000002</v>
-      </c>
-      <c r="L6" s="3">
-        <v>1.3852</v>
-      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="3"/>
       <c r="M6" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>16</v>
@@ -1242,7 +1229,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>1500</v>
@@ -1254,25 +1241,25 @@
         <v>1.3956200000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>572</v>
+        <v>587</v>
       </c>
       <c r="G8" s="1">
         <v>1500000</v>
       </c>
       <c r="H8" s="1">
-        <v>575870</v>
+        <v>590983</v>
       </c>
       <c r="I8" s="3">
-        <v>0.38390999999999997</v>
+        <v>0.39399000000000001</v>
       </c>
       <c r="J8" s="1">
         <v>10</v>
       </c>
       <c r="K8" s="3">
-        <v>1.9806699999999999</v>
+        <v>2.0233300000000001</v>
       </c>
       <c r="L8" s="3">
-        <v>1.3955900000000001</v>
+        <v>1.39554</v>
       </c>
       <c r="M8" s="1">
         <v>10</v>
@@ -1286,7 +1273,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>1500</v>
@@ -1298,25 +1285,25 @@
         <v>1.3956200000000001</v>
       </c>
       <c r="F9" s="1">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="G9" s="1">
         <v>1500000</v>
       </c>
       <c r="H9" s="1">
-        <v>197094</v>
+        <v>180570</v>
       </c>
       <c r="I9" s="3">
-        <v>0.13139999999999999</v>
+        <v>0.12038</v>
       </c>
       <c r="J9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" s="6">
-        <v>3.5939999999999999</v>
+        <v>2.7480000000000002</v>
       </c>
       <c r="L9" s="3">
-        <v>1.3643700000000001</v>
+        <v>1.3852</v>
       </c>
       <c r="M9" s="1">
         <v>10</v>
@@ -1346,7 +1333,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1">
         <v>1500</v>
@@ -1358,31 +1345,39 @@
         <v>1.3956200000000001</v>
       </c>
       <c r="F11" s="1">
-        <v>50</v>
+        <v>572</v>
       </c>
       <c r="G11" s="1">
         <v>1500000</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="3"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="H11" s="1">
+        <v>575870</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.38390999999999997</v>
+      </c>
+      <c r="J11" s="1">
+        <v>10</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.9806699999999999</v>
+      </c>
+      <c r="L11" s="3">
+        <v>1.3955900000000001</v>
+      </c>
+      <c r="M11" s="1">
+        <v>10</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="1">
         <v>1500</v>
@@ -1394,74 +1389,170 @@
         <v>1.3956200000000001</v>
       </c>
       <c r="F12" s="1">
-        <v>100</v>
+        <v>188</v>
       </c>
       <c r="G12" s="1">
         <v>1500000</v>
       </c>
       <c r="H12" s="1">
-        <v>156512</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.10434</v>
+        <v>197094</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.13139999999999999</v>
       </c>
       <c r="J12" s="1">
-        <v>37.674669999999999</v>
-      </c>
-      <c r="K12" s="3">
-        <v>37.674669999999999</v>
+        <v>4</v>
+      </c>
+      <c r="K12" s="6">
+        <v>3.5939999999999999</v>
       </c>
       <c r="L12" s="3">
-        <v>1.2782199999999999</v>
+        <v>1.3643700000000001</v>
       </c>
       <c r="M12" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="1">
         <v>1500</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D14" s="1">
         <v>1000</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E14" s="3">
         <v>1.3956200000000001</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F14" s="1">
+        <v>50</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1.3956200000000001</v>
+      </c>
+      <c r="F15" s="1">
+        <v>100</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="H15" s="1">
+        <v>156512</v>
+      </c>
+      <c r="I15" s="6">
+        <v>0.10434</v>
+      </c>
+      <c r="J15" s="1">
+        <v>37.674669999999999</v>
+      </c>
+      <c r="K15" s="3">
+        <v>37.674669999999999</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1.2782199999999999</v>
+      </c>
+      <c r="M15" s="1">
+        <v>100</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1.3956200000000001</v>
+      </c>
+      <c r="F16" s="1">
         <v>188</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G16" s="1">
         <v>1500000</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H16" s="1">
         <v>243675</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I16" s="3">
         <v>0.16245000000000001</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J16" s="1">
         <v>37.116669999999999</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K16" s="3">
         <v>37.116669999999999</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L16" s="3">
         <v>1.13178</v>
       </c>
-      <c r="M13" s="1">
+      <c r="M16" s="1">
         <v>188</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>